<commit_message>
Updated alignment files to remove KT804738 (RSIV) genome from alignments in genus and family level alignment files.
This genome was mis-aligned, likely due to a sequencing error. The same genomes was not included in the alignment at the species level (Orthogroup OG0000039)
</commit_message>
<xml_diff>
--- a/alignment_manual_changes.xlsx
+++ b/alignment_manual_changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{887E55CB-68F7-4C6E-B521-2A75E9DA7E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F381B4A3-C46D-4A38-8FB6-0A87D8588589}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="8_{887E55CB-68F7-4C6E-B521-2A75E9DA7E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64C5EF93-922B-449F-B266-C654FF3A715D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B05F01D2-BAAD-4BCF-B583-27E4851AB6BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{B05F01D2-BAAD-4BCF-B583-27E4851AB6BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Family" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="260">
   <si>
     <t>Alignment </t>
   </si>
@@ -856,6 +856,12 @@
 MF599468 (genome) 
 MF599468_Decapodiridovirus_litopenaeus1_n/a_1 
 MF599468_Decapodiridovirus_litopenaeus1_n/a_2 </t>
+  </si>
+  <si>
+    <t>Removed sequence KT804738_Megalocytivirus_pagrus1_RSIV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The second half of the sequence was miss-aligned with the other RSIV genotypes in the alignment. I could not shift the alignment to align the amino acids. </t>
   </si>
 </sst>
 </file>
@@ -934,6 +940,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1255,18 +1265,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1D177B-7F3C-499B-AB5A-90CDE1F63245}">
   <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="93.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="59.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="93.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="59.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1277,7 +1287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="405" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1288,7 +1298,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1299,7 +1309,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1310,7 +1320,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1321,7 +1331,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1332,7 +1342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1343,7 +1353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1354,7 +1364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1365,7 +1375,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1376,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1387,7 +1397,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1398,7 +1408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1409,7 +1419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1420,7 +1430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1431,7 +1441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1442,7 +1452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1453,7 +1463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1464,7 +1474,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -1475,7 +1485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -1486,7 +1496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -1497,7 +1507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -1508,7 +1518,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -1519,7 +1529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1530,7 +1540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -1541,7 +1551,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1552,7 +1562,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -1563,7 +1573,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -1574,7 +1584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -1585,7 +1595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -1596,18 +1606,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>4</v>
+        <v>258</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -1618,7 +1628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -1629,7 +1639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -1640,7 +1650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -1651,7 +1661,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -1662,7 +1672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>43</v>
       </c>
@@ -1673,7 +1683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>44</v>
       </c>
@@ -1684,7 +1694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>45</v>
       </c>
@@ -1695,7 +1705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>46</v>
       </c>
@@ -1706,7 +1716,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>47</v>
       </c>
@@ -1717,7 +1727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>49</v>
       </c>
@@ -1728,7 +1738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>50</v>
       </c>
@@ -1739,7 +1749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>51</v>
       </c>
@@ -1750,7 +1760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>52</v>
       </c>
@@ -1761,7 +1771,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>53</v>
       </c>
@@ -1772,7 +1782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>54</v>
       </c>
@@ -1783,7 +1793,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>55</v>
       </c>
@@ -1794,7 +1804,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>56</v>
       </c>
@@ -1805,7 +1815,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>57</v>
       </c>
@@ -1816,7 +1826,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>58</v>
       </c>
@@ -1827,7 +1837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>59</v>
       </c>
@@ -1838,7 +1848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>60</v>
       </c>
@@ -1849,7 +1859,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>61</v>
       </c>
@@ -1860,7 +1870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>62</v>
       </c>
@@ -1871,7 +1881,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>63</v>
       </c>
@@ -1882,7 +1892,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>64</v>
       </c>
@@ -1893,7 +1903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -1904,7 +1914,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>66</v>
       </c>
@@ -1915,7 +1925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>67</v>
       </c>
@@ -1926,7 +1936,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>68</v>
       </c>
@@ -1937,7 +1947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>69</v>
       </c>
@@ -1948,7 +1958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>70</v>
       </c>
@@ -1959,7 +1969,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>71</v>
       </c>
@@ -1970,7 +1980,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>72</v>
       </c>
@@ -1981,7 +1991,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>73</v>
       </c>
@@ -1992,7 +2002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>74</v>
       </c>
@@ -2003,7 +2013,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>75</v>
       </c>
@@ -2014,7 +2024,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>76</v>
       </c>
@@ -2025,7 +2035,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>77</v>
       </c>
@@ -2036,7 +2046,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>78</v>
       </c>
@@ -2047,7 +2057,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>79</v>
       </c>
@@ -2058,7 +2068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>80</v>
       </c>
@@ -2069,7 +2079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>81</v>
       </c>
@@ -2080,7 +2090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>82</v>
       </c>
@@ -2091,7 +2101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>83</v>
       </c>
@@ -2102,7 +2112,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>84</v>
       </c>
@@ -2113,7 +2123,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>85</v>
       </c>
@@ -2124,7 +2134,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>86</v>
       </c>
@@ -2135,7 +2145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>87</v>
       </c>
@@ -2146,7 +2156,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>88</v>
       </c>
@@ -2157,7 +2167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>89</v>
       </c>
@@ -2168,7 +2178,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>90</v>
       </c>
@@ -2179,7 +2189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>91</v>
       </c>
@@ -2190,7 +2200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>92</v>
       </c>
@@ -2201,7 +2211,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>93</v>
       </c>
@@ -2212,7 +2222,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>94</v>
       </c>
@@ -2223,7 +2233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>95</v>
       </c>
@@ -2234,7 +2244,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>96</v>
       </c>
@@ -2245,7 +2255,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>97</v>
       </c>
@@ -2256,7 +2266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>98</v>
       </c>
@@ -2267,7 +2277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>99</v>
       </c>
@@ -2278,7 +2288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>100</v>
       </c>
@@ -2289,7 +2299,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>101</v>
       </c>
@@ -2300,7 +2310,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>102</v>
       </c>
@@ -2311,7 +2321,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>103</v>
       </c>
@@ -2322,7 +2332,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>104</v>
       </c>
@@ -2333,7 +2343,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>105</v>
       </c>
@@ -2344,7 +2354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>106</v>
       </c>
@@ -2355,7 +2365,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>107</v>
       </c>
@@ -2366,7 +2376,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>108</v>
       </c>
@@ -2377,7 +2387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>109</v>
       </c>
@@ -2388,7 +2398,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>110</v>
       </c>
@@ -2399,7 +2409,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>111</v>
       </c>
@@ -2410,7 +2420,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>112</v>
       </c>
@@ -2421,7 +2431,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>113</v>
       </c>
@@ -2441,18 +2451,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0B20D4-1C93-42FE-B91A-B9F801D5DCE5}">
   <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" style="1" customWidth="1"/>
     <col min="2" max="2" width="57" style="2" customWidth="1"/>
-    <col min="3" max="3" width="62.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="62.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2463,7 +2473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>120</v>
       </c>
@@ -2474,7 +2484,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>121</v>
       </c>
@@ -2485,7 +2495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>122</v>
       </c>
@@ -2496,7 +2506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>123</v>
       </c>
@@ -2507,7 +2517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>124</v>
       </c>
@@ -2518,7 +2528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>125</v>
       </c>
@@ -2529,7 +2539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>126</v>
       </c>
@@ -2540,7 +2550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>127</v>
       </c>
@@ -2551,7 +2561,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>128</v>
       </c>
@@ -2562,7 +2572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>129</v>
       </c>
@@ -2573,7 +2583,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>130</v>
       </c>
@@ -2584,7 +2594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>131</v>
       </c>
@@ -2595,7 +2605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>132</v>
       </c>
@@ -2606,7 +2616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>133</v>
       </c>
@@ -2617,7 +2627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>134</v>
       </c>
@@ -2628,7 +2638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>135</v>
       </c>
@@ -2639,7 +2649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>136</v>
       </c>
@@ -2650,7 +2660,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>137</v>
       </c>
@@ -2661,7 +2671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>138</v>
       </c>
@@ -2672,7 +2682,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>139</v>
       </c>
@@ -2683,7 +2693,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>140</v>
       </c>
@@ -2694,7 +2704,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>141</v>
       </c>
@@ -2705,7 +2715,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>142</v>
       </c>
@@ -2716,18 +2726,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>4</v>
+      <c r="B25" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>144</v>
       </c>
@@ -2738,7 +2748,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>145</v>
       </c>
@@ -2749,7 +2759,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>146</v>
       </c>
@@ -2760,7 +2770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>147</v>
       </c>
@@ -2771,7 +2781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>148</v>
       </c>
@@ -2782,7 +2792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>149</v>
       </c>
@@ -2793,7 +2803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>150</v>
       </c>
@@ -2804,7 +2814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>151</v>
       </c>
@@ -2815,7 +2825,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>152</v>
       </c>
@@ -2826,7 +2836,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>153</v>
       </c>
@@ -2837,7 +2847,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>154</v>
       </c>
@@ -2848,7 +2858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>155</v>
       </c>
@@ -2859,7 +2869,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>156</v>
       </c>
@@ -2870,7 +2880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>157</v>
       </c>
@@ -2881,7 +2891,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>158</v>
       </c>
@@ -2892,7 +2902,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>159</v>
       </c>
@@ -2903,7 +2913,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>160</v>
       </c>
@@ -2914,7 +2924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>161</v>
       </c>
@@ -2925,7 +2935,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>162</v>
       </c>
@@ -2936,7 +2946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>163</v>
       </c>
@@ -2947,7 +2957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>164</v>
       </c>
@@ -2958,7 +2968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>165</v>
       </c>
@@ -2969,7 +2979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>166</v>
       </c>
@@ -2980,7 +2990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>167</v>
       </c>
@@ -2991,7 +3001,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>168</v>
       </c>
@@ -3002,7 +3012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>169</v>
       </c>
@@ -3013,7 +3023,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>170</v>
       </c>
@@ -3024,57 +3034,57 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>181</v>
       </c>
@@ -3085,7 +3095,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>182</v>
       </c>
@@ -3096,7 +3106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>183</v>
       </c>
@@ -3107,7 +3117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>184</v>
       </c>
@@ -3118,7 +3128,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>185</v>
       </c>
@@ -3129,7 +3139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>186</v>
       </c>
@@ -3140,7 +3150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>187</v>
       </c>
@@ -3151,7 +3161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>188</v>
       </c>
@@ -3162,7 +3172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>189</v>
       </c>
@@ -3173,7 +3183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>190</v>
       </c>
@@ -3184,7 +3194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>191</v>
       </c>
@@ -3195,7 +3205,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>192</v>
       </c>
@@ -3206,7 +3216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>193</v>
       </c>
@@ -3217,7 +3227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>194</v>
       </c>
@@ -3228,7 +3238,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>195</v>
       </c>
@@ -3239,7 +3249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>196</v>
       </c>
@@ -3250,7 +3260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>197</v>
       </c>
@@ -3261,7 +3271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>198</v>
       </c>
@@ -3272,7 +3282,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>199</v>
       </c>
@@ -3283,7 +3293,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>200</v>
       </c>
@@ -3294,7 +3304,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>201</v>
       </c>
@@ -3305,7 +3315,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>202</v>
       </c>
@@ -3316,7 +3326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>203</v>
       </c>
@@ -3327,7 +3337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>204</v>
       </c>
@@ -3338,7 +3348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>205</v>
       </c>
@@ -3349,7 +3359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>206</v>
       </c>
@@ -3360,7 +3370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>207</v>
       </c>
@@ -3371,7 +3381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>208</v>
       </c>
@@ -3382,7 +3392,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>209</v>
       </c>
@@ -3393,7 +3403,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>210</v>
       </c>
@@ -3404,7 +3414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>211</v>
       </c>
@@ -3415,7 +3425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>212</v>
       </c>
@@ -3426,7 +3436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>213</v>
       </c>
@@ -3437,7 +3447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>214</v>
       </c>
@@ -3448,7 +3458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>215</v>
       </c>
@@ -3459,7 +3469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>216</v>
       </c>
@@ -3470,7 +3480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>217</v>
       </c>
@@ -3481,7 +3491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>218</v>
       </c>
@@ -3492,7 +3502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>219</v>
       </c>
@@ -3503,7 +3513,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>220</v>
       </c>
@@ -3514,7 +3524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>221</v>
       </c>
@@ -3525,7 +3535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>222</v>
       </c>
@@ -3536,7 +3546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>223</v>
       </c>
@@ -3547,7 +3557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>224</v>
       </c>
@@ -3558,7 +3568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>225</v>
       </c>
@@ -3569,7 +3579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>226</v>
       </c>
@@ -3580,7 +3590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>227</v>
       </c>
@@ -3591,7 +3601,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>228</v>
       </c>
@@ -3602,7 +3612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>229</v>
       </c>
@@ -3613,7 +3623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>230</v>
       </c>
@@ -3624,7 +3634,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>231</v>
       </c>
@@ -3635,7 +3645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>232</v>
       </c>
@@ -3646,7 +3656,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>233</v>
       </c>
@@ -3657,7 +3667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>234</v>
       </c>
@@ -3681,14 +3691,14 @@
       <selection activeCell="A116" sqref="A2:A116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="77" style="1" customWidth="1"/>
-    <col min="3" max="3" width="59.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="59.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3699,7 +3709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>120</v>
       </c>
@@ -3710,7 +3720,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>121</v>
       </c>
@@ -3721,7 +3731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>122</v>
       </c>
@@ -3732,7 +3742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>123</v>
       </c>
@@ -3743,7 +3753,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>124</v>
       </c>
@@ -3754,7 +3764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>125</v>
       </c>
@@ -3765,7 +3775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>126</v>
       </c>
@@ -3776,7 +3786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>127</v>
       </c>
@@ -3787,7 +3797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>128</v>
       </c>
@@ -3798,7 +3808,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>129</v>
       </c>
@@ -3809,7 +3819,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>130</v>
       </c>
@@ -3820,7 +3830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>131</v>
       </c>
@@ -3831,7 +3841,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>132</v>
       </c>
@@ -3842,7 +3852,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>133</v>
       </c>
@@ -3853,7 +3863,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>134</v>
       </c>
@@ -3864,7 +3874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>135</v>
       </c>
@@ -3875,7 +3885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>136</v>
       </c>
@@ -3886,7 +3896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>137</v>
       </c>
@@ -3897,7 +3907,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>138</v>
       </c>
@@ -3908,7 +3918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>139</v>
       </c>
@@ -3919,7 +3929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>140</v>
       </c>
@@ -3930,7 +3940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>141</v>
       </c>
@@ -3941,7 +3951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>142</v>
       </c>
@@ -3952,7 +3962,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>143</v>
       </c>
@@ -3963,7 +3973,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>144</v>
       </c>
@@ -3974,7 +3984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>145</v>
       </c>
@@ -3985,7 +3995,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>146</v>
       </c>
@@ -3996,7 +4006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>147</v>
       </c>
@@ -4007,7 +4017,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>148</v>
       </c>
@@ -4018,7 +4028,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>149</v>
       </c>
@@ -4029,7 +4039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>150</v>
       </c>
@@ -4040,7 +4050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>151</v>
       </c>
@@ -4051,7 +4061,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>152</v>
       </c>
@@ -4062,7 +4072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>153</v>
       </c>
@@ -4073,7 +4083,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>154</v>
       </c>
@@ -4084,7 +4094,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>155</v>
       </c>
@@ -4095,7 +4105,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>156</v>
       </c>
@@ -4106,7 +4116,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>157</v>
       </c>
@@ -4117,7 +4127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>158</v>
       </c>
@@ -4128,7 +4138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>159</v>
       </c>
@@ -4139,7 +4149,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>160</v>
       </c>
@@ -4150,7 +4160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>161</v>
       </c>
@@ -4161,7 +4171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>162</v>
       </c>
@@ -4172,7 +4182,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>163</v>
       </c>
@@ -4183,7 +4193,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>164</v>
       </c>
@@ -4194,7 +4204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>165</v>
       </c>
@@ -4205,7 +4215,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>166</v>
       </c>
@@ -4216,7 +4226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>167</v>
       </c>
@@ -4227,7 +4237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>168</v>
       </c>
@@ -4238,7 +4248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>169</v>
       </c>
@@ -4249,7 +4259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>170</v>
       </c>
@@ -4260,7 +4270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>171</v>
       </c>
@@ -4268,7 +4278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>172</v>
       </c>
@@ -4276,7 +4286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>173</v>
       </c>
@@ -4284,7 +4294,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>174</v>
       </c>
@@ -4292,7 +4302,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>175</v>
       </c>
@@ -4300,7 +4310,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>176</v>
       </c>
@@ -4308,7 +4318,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>177</v>
       </c>
@@ -4316,7 +4326,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>178</v>
       </c>
@@ -4324,7 +4334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>179</v>
       </c>
@@ -4332,7 +4342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>180</v>
       </c>
@@ -4340,7 +4350,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>181</v>
       </c>
@@ -4351,7 +4361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>182</v>
       </c>
@@ -4362,7 +4372,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>183</v>
       </c>
@@ -4373,7 +4383,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>184</v>
       </c>
@@ -4384,7 +4394,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>185</v>
       </c>
@@ -4395,7 +4405,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>186</v>
       </c>
@@ -4406,7 +4416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>187</v>
       </c>
@@ -4417,7 +4427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>188</v>
       </c>
@@ -4428,7 +4438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>189</v>
       </c>
@@ -4439,7 +4449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>190</v>
       </c>
@@ -4450,7 +4460,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>191</v>
       </c>
@@ -4461,7 +4471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>192</v>
       </c>
@@ -4472,7 +4482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>193</v>
       </c>
@@ -4483,7 +4493,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>194</v>
       </c>
@@ -4494,7 +4504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>195</v>
       </c>
@@ -4505,7 +4515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>196</v>
       </c>
@@ -4516,7 +4526,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>197</v>
       </c>
@@ -4527,7 +4537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>198</v>
       </c>
@@ -4538,7 +4548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>199</v>
       </c>
@@ -4549,7 +4559,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>200</v>
       </c>
@@ -4560,7 +4570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>201</v>
       </c>
@@ -4571,7 +4581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>202</v>
       </c>
@@ -4582,7 +4592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>203</v>
       </c>
@@ -4593,7 +4603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>204</v>
       </c>
@@ -4604,7 +4614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>205</v>
       </c>
@@ -4615,7 +4625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>206</v>
       </c>
@@ -4626,7 +4636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>207</v>
       </c>
@@ -4637,7 +4647,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>208</v>
       </c>
@@ -4648,7 +4658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>209</v>
       </c>
@@ -4659,7 +4669,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>210</v>
       </c>
@@ -4670,7 +4680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>211</v>
       </c>
@@ -4681,7 +4691,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>212</v>
       </c>
@@ -4692,7 +4702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>213</v>
       </c>
@@ -4703,7 +4713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>214</v>
       </c>
@@ -4714,7 +4724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>215</v>
       </c>
@@ -4725,7 +4735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>216</v>
       </c>
@@ -4736,7 +4746,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>217</v>
       </c>
@@ -4747,7 +4757,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>218</v>
       </c>
@@ -4758,7 +4768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>219</v>
       </c>
@@ -4769,7 +4779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>220</v>
       </c>
@@ -4780,7 +4790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>221</v>
       </c>
@@ -4791,7 +4801,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>222</v>
       </c>
@@ -4802,7 +4812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>223</v>
       </c>
@@ -4813,7 +4823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>224</v>
       </c>
@@ -4824,7 +4834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>225</v>
       </c>
@@ -4835,7 +4845,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>226</v>
       </c>
@@ -4846,7 +4856,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>227</v>
       </c>
@@ -4857,7 +4867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>228</v>
       </c>
@@ -4868,7 +4878,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>229</v>
       </c>
@@ -4879,7 +4889,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>230</v>
       </c>
@@ -4890,7 +4900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>231</v>
       </c>
@@ -4901,7 +4911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>232</v>
       </c>
@@ -4912,7 +4922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>233</v>
       </c>
@@ -4923,7 +4933,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>234</v>
       </c>

</xml_diff>

<commit_message>
Updates alignments to remove taxa with branch lengths >0.9.
</commit_message>
<xml_diff>
--- a/alignment_manual_changes.xlsx
+++ b/alignment_manual_changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{887E55CB-68F7-4C6E-B521-2A75E9DA7E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64C5EF93-922B-449F-B266-C654FF3A715D}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="8_{887E55CB-68F7-4C6E-B521-2A75E9DA7E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{916CF8FD-0346-426B-B4DD-E13C7917FCE6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{B05F01D2-BAAD-4BCF-B583-27E4851AB6BB}"/>
+    <workbookView xWindow="1944" yWindow="2208" windowWidth="17280" windowHeight="10044" xr2:uid="{B05F01D2-BAAD-4BCF-B583-27E4851AB6BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Family" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="268">
   <si>
     <t>Alignment </t>
   </si>
@@ -862,6 +862,30 @@
   </si>
   <si>
     <t xml:space="preserve">The second half of the sequence was miss-aligned with the other RSIV genotypes in the alignment. I could not shift the alignment to align the amino acids. </t>
+  </si>
+  <si>
+    <t>Branch length 0.9054</t>
+  </si>
+  <si>
+    <t>Removed LS484712_Daphniairidovirus_daphnia1</t>
+  </si>
+  <si>
+    <t>Branch length 1.339</t>
+  </si>
+  <si>
+    <t>Branch length 0.9578</t>
+  </si>
+  <si>
+    <t>Branch length 1.181</t>
+  </si>
+  <si>
+    <t>Branch length 1.108</t>
+  </si>
+  <si>
+    <t>Removed AY894343_Megalocytivirus_pagrus1_RSIV</t>
+  </si>
+  <si>
+    <t>Branch length 1.049</t>
   </si>
 </sst>
 </file>
@@ -1265,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1D177B-7F3C-499B-AB5A-90CDE1F63245}">
   <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1358,10 +1382,10 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>261</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1402,10 +1426,10 @@
         <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>4</v>
+        <v>261</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>5</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1413,10 +1437,10 @@
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>4</v>
+        <v>261</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>5</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1446,10 +1470,10 @@
         <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>4</v>
+        <v>261</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>5</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -1490,10 +1514,10 @@
         <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>4</v>
+        <v>261</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>5</v>
+        <v>265</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1622,10 +1646,10 @@
         <v>38</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>4</v>
+        <v>266</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>5</v>
+        <v>267</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -2451,7 +2475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0B20D4-1C93-42FE-B91A-B9F801D5DCE5}">
   <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updating spreadsheets following quality check
</commit_message>
<xml_diff>
--- a/alignment_manual_changes.xlsx
+++ b/alignment_manual_changes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="8_{887E55CB-68F7-4C6E-B521-2A75E9DA7E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21B1C416-D9F3-489D-A055-66D1EED0C1AB}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="8_{887E55CB-68F7-4C6E-B521-2A75E9DA7E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3451FBC9-D9C8-401B-8C08-27EC123ED7FF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B05F01D2-BAAD-4BCF-B583-27E4851AB6BB}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="285">
   <si>
     <t>Alignment </t>
   </si>
@@ -816,13 +816,6 @@
     <t>KF938901 Has two genes (next to one another in genome) which I think should be together. There are two in this Orthogroup and the other starts where the other one begins. I have labelled them: 
 KF938901_Chloriridovirus_anopheles1_n/a_1, and  
 KF938901_Chloriridovirus_anopheles1_n/a_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Removed 
-Both sequences for HF920637. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Removed KX643370_Lymphocystivirus_sparus1_n/a 2: </t>
   </si>
   <si>
     <t>HF920637 (genome) 
@@ -865,9 +858,6 @@
     <t>Branch length 0.9054</t>
   </si>
   <si>
-    <t>Removed LS484712_Daphniairidovirus_daphnia1</t>
-  </si>
-  <si>
     <t>Branch length 1.339</t>
   </si>
   <si>
@@ -884,9 +874,6 @@
   </si>
   <si>
     <t xml:space="preserve">Two iridovirus sequences from one genome (HF920637) are included. Both with large gaps in the sequences. </t>
-  </si>
-  <si>
-    <t>Removed AY521625_Megalocytivirus_pagrus1_RSIV</t>
   </si>
   <si>
     <t>Both KT804738_Megalocytivirus_pagrus1_RSIV and AY894343_Megalocytivirus_pagrus1_RSIV have sections which no other genome has. Unsure if sequencing error. They were sequences in 2002 and 2006 in different labs in different countries. One was in groper and the other in barramundi.  </t>
@@ -1025,6 +1012,152 @@
   </si>
   <si>
     <t>Branch length to clade 3.3504</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No longer considered core gene. Considered a phylogenetically useful gene. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Removed 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">KX643370_Lymphocystivirus_sparus1_n/a 2: </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Removed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Both sequences for HF920637. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Removed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LS484712_Daphniairidovirus_daphnia1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Removed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> LS484712_Daphniairidovirus_daphnia1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Removed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sequence KT804738_Megalocytivirus_pagrus1_RSIV</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Removed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> AY521625_Megalocytivirus_pagrus1_RSIV</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1074,7 +1207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1089,6 +1222,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1427,11 +1566,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1D177B-7F3C-499B-AB5A-90CDE1F63245}">
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1441,49 +1581,53 @@
     <col min="3" max="3" width="59.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="93.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="45.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="405" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="405" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>252</v>
+      <c r="B3" s="2" t="s">
+        <v>279</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1494,24 +1638,30 @@
         <v>246</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>251</v>
+        <v>280</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1522,7 +1672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1533,18 +1683,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>258</v>
+        <v>281</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1555,7 +1708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1566,7 +1719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1578,35 +1731,41 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>258</v>
+        <v>281</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1617,13 +1776,16 @@
         <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1634,18 +1796,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1656,13 +1821,16 @@
         <v>5</v>
       </c>
       <c r="D17" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1673,7 +1841,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -1684,18 +1852,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -1706,7 +1877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -1717,7 +1888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -1728,7 +1899,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1739,7 +1910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -1750,7 +1921,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1761,13 +1932,16 @@
         <v>247</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E26" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -1778,7 +1952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -1789,7 +1963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -1800,7 +1974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -1811,26 +1985,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>255</v>
+        <v>283</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>265</v>
+        <v>284</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2936,10 +3110,10 @@
         <v>143</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -3387,10 +3561,10 @@
         <v>184</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates after including new megalocytivirus genome European chub iridovirus
</commit_message>
<xml_diff>
--- a/alignment_manual_changes.xlsx
+++ b/alignment_manual_changes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="8_{887E55CB-68F7-4C6E-B521-2A75E9DA7E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3451FBC9-D9C8-401B-8C08-27EC123ED7FF}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="8_{887E55CB-68F7-4C6E-B521-2A75E9DA7E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A161095-56E7-41F7-AF4A-C3069EF96957}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B05F01D2-BAAD-4BCF-B583-27E4851AB6BB}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11325" xr2:uid="{B05F01D2-BAAD-4BCF-B583-27E4851AB6BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Family" sheetId="3" r:id="rId1"/>
@@ -805,14 +805,6 @@
  KF938901_Chloriridovirus_anopheles1_n/a</t>
   </si>
   <si>
-    <t xml:space="preserve">KF938901 (genome) 
-KF938901_Chloriridovirus_anopheles1_n/a_1 
-Deleted section at positions 952-1626 (32aa and 643 gaps deleted) 
- KF938901_Chloriridovirus_anopheles1_n/a_2 
-Deleted section at positions 1-1035 (0aa and 1025 gaps deleted) 
-Whole sequence moved left when gaps deleted. I moved it back to the start position 1035.  </t>
-  </si>
-  <si>
     <t>KF938901 Has two genes (next to one another in genome) which I think should be together. There are two in this Orthogroup and the other starts where the other one begins. I have labelled them: 
 KF938901_Chloriridovirus_anopheles1_n/a_1, and  
 KF938901_Chloriridovirus_anopheles1_n/a_</t>
@@ -1158,6 +1150,17 @@
       </rPr>
       <t xml:space="preserve"> AY521625_Megalocytivirus_pagrus1_RSIV</t>
     </r>
+  </si>
+  <si>
+    <t>KF938901 (genome) 
+KF938901_Chloriridovirus_anopheles1_n/a_1 
+Deleted section at positions 952-1626 (32aa and 643 gaps deleted) 
+ KF938901_Chloriridovirus_anopheles1_n/a_2 
+Deleted section at positions 1-1035 (0aa and 1025 gaps deleted) 
+Whole sequence moved left when gaps deleted. I moved it back to the start position 1035.
+Combined  KF938901_Chloriridovirus_anopheles1_n/a_1 and KF938901_Chloriridovirus_anopheles1_n/a_2. The sequence appended _2 was moved to begin at position 1035 in the sequence appending _1, where only gaps existed. The section moved was 464 amino acids in length and included 128 gaps. 
+Removed  KF938901_Chloriridovirus_anopheles1_n/a_2 
+Updated the name of the seqeunce appended _2 to remove the _2. The sequence name is now KF938901_Chloriridovirus_anopheles1_n/a.</t>
   </si>
 </sst>
 </file>
@@ -1568,10 +1571,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1D177B-7F3C-499B-AB5A-90CDE1F63245}">
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="B26" sqref="B26"/>
+      <selection pane="topRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1589,19 +1592,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>266</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="405" x14ac:dyDescent="0.25">
@@ -1609,10 +1612,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>252</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -1621,7 +1624,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>244</v>
@@ -1638,13 +1641,13 @@
         <v>246</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1652,13 +1655,13 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1688,13 +1691,13 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1719,15 +1722,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>250</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -1736,19 +1739,19 @@
         <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1756,13 +1759,13 @@
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1776,13 +1779,13 @@
         <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>272</v>
-      </c>
       <c r="F14" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1801,13 +1804,13 @@
         <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1821,13 +1824,13 @@
         <v>5</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1857,13 +1860,13 @@
         <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1932,13 +1935,13 @@
         <v>247</v>
       </c>
       <c r="D26" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E26" t="s">
         <v>275</v>
       </c>
-      <c r="E26" t="s">
-        <v>276</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1990,10 +1993,10 @@
         <v>37</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2001,10 +2004,10 @@
         <v>38</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3110,10 +3113,10 @@
         <v>143</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -3561,10 +3564,10 @@
         <v>184</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates following review of alignments and trees with sequences included for newly-added genome of European chub iridovirus
</commit_message>
<xml_diff>
--- a/alignment_manual_changes.xlsx
+++ b/alignment_manual_changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="8_{887E55CB-68F7-4C6E-B521-2A75E9DA7E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A161095-56E7-41F7-AF4A-C3069EF96957}"/>
+  <xr:revisionPtr revIDLastSave="200" documentId="8_{887E55CB-68F7-4C6E-B521-2A75E9DA7E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A720C2D-A6F5-4F82-927F-C679BF45B521}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11325" xr2:uid="{B05F01D2-BAAD-4BCF-B583-27E4851AB6BB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B05F01D2-BAAD-4BCF-B583-27E4851AB6BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Family" sheetId="3" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="295">
   <si>
     <t>Alignment </t>
   </si>
@@ -192,9 +192,6 @@
     <t>G0000039 </t>
   </si>
   <si>
-    <t>Remove KT804738_Megalocytivirus_pagrus1_RSIV </t>
-  </si>
-  <si>
     <t>G0000040 </t>
   </si>
   <si>
@@ -390,18 +387,12 @@
     <t>G0000113 </t>
   </si>
   <si>
-    <t>Removed sequence OQ513807_Megalocytivirus_pagrus1_ISKNV </t>
-  </si>
-  <si>
     <t xml:space="preserve">Sequence OQ513807_Megalocytivirus_pagrus1_ISKNV is quite different from all other sequences in the alignment. It has large sections of gaps inserted where no other sequence does. I assume this is a result of a sequencing error. </t>
   </si>
   <si>
     <t>Seqeuence OQ513807_Megalocytivirus_pagrus1_ISKNV is quite different from other sequences in the alignment. It has large sections of gaps inserted where no other sequence in the genome does. I assume this is due to a sequencing error.  </t>
   </si>
   <si>
-    <t>Removed BD143114_Megalocytivirus_pagrus1_RSIV </t>
-  </si>
-  <si>
     <t>BD143114 sequence is similar to all other taxa for the first half but the last quarter is completely different. I assume this is due to a sequencing error.</t>
   </si>
   <si>
@@ -756,23 +747,13 @@
     <t>Removed sequence MN562489_Megalocytivirus_lates1_SDDV </t>
   </si>
   <si>
-    <t>Removed 23043610003_Megalocytivirus_pagrus1_ISKNV due to assumed sequencing error.  </t>
-  </si>
-  <si>
     <t>The last ¼ of the sequence for 23043610003_Megalocytivirus_pagrus1_ISKNV is different to all the others which is highly unusual given its ISKNV.  </t>
   </si>
   <si>
-    <t>Deleted OQ513807_Megalocytivirus_pagrus1_ISKNV </t>
-  </si>
-  <si>
     <t xml:space="preserve">Sequence OQ513807_Megalocytivirus_pagrus1_ISKNV was significantly different to other sequences. </t>
   </si>
   <si>
     <t>Seqeuence OQ513807_Megalocytivirus_pagrus1_ISKNV was significantly different to all other sequences.</t>
-  </si>
-  <si>
-    <t>Removed  PQ335173_PQ335174_Threespine_stickleback_iridovirus_TSIV. 
-Renamed PQ335173_PQ335174_Threespine_stickleback_iridovirus_TSIV 2, to  PQ335173_PQ335174_Threespine_stickleback_iridovirus_TSIV. </t>
   </si>
   <si>
     <t xml:space="preserve">Two sequences included for: 
@@ -869,9 +850,6 @@
   </si>
   <si>
     <t>Both KT804738_Megalocytivirus_pagrus1_RSIV and AY894343_Megalocytivirus_pagrus1_RSIV have sections which no other genome has. Unsure if sequencing error. They were sequences in 2002 and 2006 in different labs in different countries. One was in groper and the other in barramundi.  </t>
-  </si>
-  <si>
-    <t>Removed KT804738_Megalocytivirus_pagrus1_RSIV and  AY894343_Megalocytivirus_pagrus1_RSIV</t>
   </si>
   <si>
     <t>Change before IQTREE gene trees were generated</t>
@@ -1161,6 +1139,325 @@
 Combined  KF938901_Chloriridovirus_anopheles1_n/a_1 and KF938901_Chloriridovirus_anopheles1_n/a_2. The sequence appended _2 was moved to begin at position 1035 in the sequence appending _1, where only gaps existed. The section moved was 464 amino acids in length and included 128 gaps. 
 Removed  KF938901_Chloriridovirus_anopheles1_n/a_2 
 Updated the name of the seqeunce appended _2 to remove the _2. The sequence name is now KF938901_Chloriridovirus_anopheles1_n/a.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Removed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> LS484712_Daphniairidovirus_daphnia1_n/a</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Removed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MF599468_Decapodiridovirus_litopenaeus1_n/a</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> Branch length 2.193. This branch length was identified on the gene tree following the inclusion of European chub iridovirus.</t>
+  </si>
+  <si>
+    <t>Branch length 2.3792. This branch length was identified on the gene tree following the inclusion of European chub iridovirus.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Removed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> MK637631_European_chub_iridovirus_ECIV
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Removed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> KX643370_Lymphocystivirus_sparus1_n/a
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Removed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MN803438_Lymphocystivirus_micropogonias1_n/a</t>
+    </r>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>MK637631_European_chub_iridovirus_ECIV did not align. I could not edit the alignment to improve it. 
+Both of the following sequences did not align well at all. This was observed visually in the alignment, as well as in the gene tree generated with iqtree. This was observed after european chub iridovirus was included in the alignments. Although, the sequences appear to not have aligned well in the previous alignment also (generated prior to the addition of european chub iridovirus). 
+KX643370_Lymphocystivirus_sparus1_n/a
+MN803438_Lymphocystivirus_micropogonias1_n/a</t>
+  </si>
+  <si>
+    <t>The second half of the sequence was miss-aligned with the other RSIV genotypes in the alignment. I could not shift the alignment to align the amino acids</t>
+  </si>
+  <si>
+    <t>MF599468_Decapodiridovirus_litopenaeus1_n/a on branch with length 1.8204 and clearly did not align well in multiple sequence alignment. I could not amend the alignment with manual edits.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Removed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>23043610003_Megalocytivirus_pagrus1_ISKNV due to assumed sequencing error.  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Removed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KT804738_Megalocytivirus_pagrus1_RSIV and  AY894343_Megalocytivirus_pagrus1_RSIV</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Removed  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PQ335173_PQ335174_Threespine_stickleback_iridovirus_TSIV. 
+Renamed PQ335173_PQ335174_Threespine_stickleback_iridovirus_TSIV 2, to  PQ335173_PQ335174_Threespine_stickleback_iridovirus_TSIV. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Removed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OQ513807_Megalocytivirus_pagrus1_ISKNV </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Removed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> OQ513807_Megalocytivirus_pagrus1_ISKNV </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Remove</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> KT804738_Megalocytivirus_pagrus1_RSIV </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Removed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> BD143114_Megalocytivirus_pagrus1_RSIV </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Removed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> OQ513807_Megalocytivirus_pagrus1_ISKNV </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1571,10 +1868,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1D177B-7F3C-499B-AB5A-90CDE1F63245}">
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="B8" sqref="B8"/>
+      <selection pane="topRight" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1592,19 +1889,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="405" x14ac:dyDescent="0.25">
@@ -1612,10 +1909,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -1624,10 +1921,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1635,19 +1932,19 @@
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1655,13 +1952,13 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1691,13 +1988,13 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1708,7 +2005,13 @@
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>5</v>
+        <v>283</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1727,10 +2030,10 @@
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -1739,19 +2042,19 @@
         <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1759,13 +2062,13 @@
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1779,13 +2082,13 @@
         <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1804,13 +2107,13 @@
         <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1824,24 +2127,24 @@
         <v>5</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>5</v>
+      <c r="D18" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1860,13 +2163,13 @@
         <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1929,19 +2232,19 @@
         <v>32</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="E26" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1977,7 +2280,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -1985,18 +2288,30 @@
         <v>4</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>253</v>
+      <c r="B31" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2004,10 +2319,10 @@
         <v>38</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2111,7 +2426,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>4</v>
@@ -2122,7 +2437,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>4</v>
@@ -2133,7 +2448,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>4</v>
@@ -2144,7 +2459,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>4</v>
@@ -2155,7 +2470,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>4</v>
@@ -2166,7 +2481,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>4</v>
@@ -2177,7 +2492,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>4</v>
@@ -2188,7 +2503,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>4</v>
@@ -2199,7 +2514,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>4</v>
@@ -2210,7 +2525,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>4</v>
@@ -2221,7 +2536,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>4</v>
@@ -2232,7 +2547,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>4</v>
@@ -2243,7 +2558,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>4</v>
@@ -2254,7 +2569,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>4</v>
@@ -2265,7 +2580,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>4</v>
@@ -2276,7 +2591,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>4</v>
@@ -2287,7 +2602,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>4</v>
@@ -2298,7 +2613,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>4</v>
@@ -2309,7 +2624,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>4</v>
@@ -2320,7 +2635,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>4</v>
@@ -2331,7 +2646,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>4</v>
@@ -2342,7 +2657,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>4</v>
@@ -2353,7 +2668,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>4</v>
@@ -2364,7 +2679,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>4</v>
@@ -2375,7 +2690,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>4</v>
@@ -2386,7 +2701,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>4</v>
@@ -2397,7 +2712,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>4</v>
@@ -2408,7 +2723,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>4</v>
@@ -2419,7 +2734,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>4</v>
@@ -2430,7 +2745,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>4</v>
@@ -2441,7 +2756,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>4</v>
@@ -2452,7 +2767,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>4</v>
@@ -2463,7 +2778,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>4</v>
@@ -2474,7 +2789,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>4</v>
@@ -2485,7 +2800,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>4</v>
@@ -2496,7 +2811,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>4</v>
@@ -2507,7 +2822,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>4</v>
@@ -2518,7 +2833,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>4</v>
@@ -2529,7 +2844,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>4</v>
@@ -2540,7 +2855,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>4</v>
@@ -2551,7 +2866,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>4</v>
@@ -2562,7 +2877,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>4</v>
@@ -2573,7 +2888,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>4</v>
@@ -2584,7 +2899,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>4</v>
@@ -2595,7 +2910,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>4</v>
@@ -2606,7 +2921,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>4</v>
@@ -2617,7 +2932,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>4</v>
@@ -2628,7 +2943,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>4</v>
@@ -2639,7 +2954,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>4</v>
@@ -2650,7 +2965,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>4</v>
@@ -2661,7 +2976,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>4</v>
@@ -2672,7 +2987,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>4</v>
@@ -2683,7 +2998,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>4</v>
@@ -2694,7 +3009,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>4</v>
@@ -2705,7 +3020,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>4</v>
@@ -2716,7 +3031,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>4</v>
@@ -2727,7 +3042,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>4</v>
@@ -2738,7 +3053,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>4</v>
@@ -2749,7 +3064,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>4</v>
@@ -2760,7 +3075,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>4</v>
@@ -2771,7 +3086,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>4</v>
@@ -2782,7 +3097,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>4</v>
@@ -2793,7 +3108,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>4</v>
@@ -2804,7 +3119,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>4</v>
@@ -2815,7 +3130,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>4</v>
@@ -2833,8 +3148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0B20D4-1C93-42FE-B91A-B9F801D5DCE5}">
   <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52:C62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2857,18 +3172,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -2879,7 +3194,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -2890,7 +3205,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -2901,7 +3216,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -2912,7 +3227,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -2923,7 +3238,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
@@ -2934,7 +3249,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>4</v>
@@ -2945,7 +3260,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
@@ -2956,7 +3271,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
@@ -2967,7 +3282,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>4</v>
@@ -2978,7 +3293,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>4</v>
@@ -2989,7 +3304,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>4</v>
@@ -3000,7 +3315,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>4</v>
@@ -3011,7 +3326,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>4</v>
@@ -3022,7 +3337,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>4</v>
@@ -3033,7 +3348,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>4</v>
@@ -3044,7 +3359,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>4</v>
@@ -3055,7 +3370,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>4</v>
@@ -3066,7 +3381,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>4</v>
@@ -3077,7 +3392,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>4</v>
@@ -3088,7 +3403,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>4</v>
@@ -3099,7 +3414,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>4</v>
@@ -3110,18 +3425,18 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>4</v>
@@ -3132,7 +3447,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>4</v>
@@ -3143,7 +3458,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>4</v>
@@ -3154,7 +3469,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>4</v>
@@ -3165,7 +3480,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>4</v>
@@ -3176,7 +3491,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>4</v>
@@ -3187,7 +3502,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>4</v>
@@ -3198,7 +3513,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>4</v>
@@ -3209,7 +3524,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>4</v>
@@ -3220,7 +3535,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>4</v>
@@ -3231,7 +3546,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>4</v>
@@ -3242,7 +3557,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>4</v>
@@ -3253,7 +3568,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>4</v>
@@ -3264,7 +3579,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>4</v>
@@ -3275,7 +3590,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>4</v>
@@ -3286,7 +3601,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>4</v>
@@ -3297,7 +3612,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>4</v>
@@ -3308,7 +3623,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>4</v>
@@ -3319,7 +3634,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>4</v>
@@ -3330,7 +3645,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>4</v>
@@ -3341,7 +3656,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>4</v>
@@ -3352,7 +3667,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>4</v>
@@ -3363,7 +3678,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>4</v>
@@ -3374,7 +3689,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>4</v>
@@ -3385,7 +3700,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>4</v>
@@ -3396,7 +3711,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>4</v>
@@ -3407,7 +3722,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>4</v>
@@ -3418,7 +3733,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>4</v>
@@ -3429,7 +3744,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>4</v>
@@ -3440,7 +3755,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>4</v>
@@ -3451,7 +3766,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>4</v>
@@ -3462,7 +3777,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>4</v>
@@ -3473,7 +3788,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>4</v>
@@ -3484,7 +3799,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>4</v>
@@ -3495,7 +3810,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>4</v>
@@ -3506,7 +3821,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>4</v>
@@ -3517,7 +3832,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>4</v>
@@ -3528,18 +3843,18 @@
     </row>
     <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>236</v>
+        <v>287</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>4</v>
@@ -3550,7 +3865,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>4</v>
@@ -3561,18 +3876,18 @@
     </row>
     <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>262</v>
+        <v>288</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>4</v>
@@ -3583,7 +3898,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>4</v>
@@ -3594,7 +3909,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>4</v>
@@ -3605,7 +3920,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>4</v>
@@ -3616,7 +3931,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>4</v>
@@ -3627,7 +3942,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>4</v>
@@ -3638,7 +3953,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>4</v>
@@ -3649,7 +3964,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>4</v>
@@ -3660,7 +3975,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>4</v>
@@ -3671,7 +3986,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>4</v>
@@ -3682,7 +3997,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>4</v>
@@ -3693,7 +4008,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>4</v>
@@ -3704,7 +4019,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>4</v>
@@ -3715,7 +4030,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>4</v>
@@ -3726,7 +4041,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>4</v>
@@ -3737,7 +4052,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>4</v>
@@ -3748,18 +4063,18 @@
     </row>
     <row r="83" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>241</v>
+        <v>289</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>4</v>
@@ -3770,7 +4085,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>4</v>
@@ -3781,7 +4096,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>4</v>
@@ -3792,7 +4107,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>4</v>
@@ -3803,7 +4118,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>4</v>
@@ -3814,7 +4129,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>4</v>
@@ -3825,7 +4140,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>4</v>
@@ -3836,7 +4151,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>4</v>
@@ -3847,7 +4162,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>4</v>
@@ -3858,7 +4173,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>4</v>
@@ -3869,7 +4184,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>4</v>
@@ -3880,7 +4195,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>4</v>
@@ -3891,7 +4206,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>4</v>
@@ -3902,7 +4217,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>4</v>
@@ -3913,7 +4228,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>4</v>
@@ -3924,7 +4239,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>4</v>
@@ -3935,7 +4250,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>4</v>
@@ -3946,7 +4261,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>4</v>
@@ -3957,7 +4272,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>4</v>
@@ -3968,7 +4283,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>4</v>
@@ -3979,7 +4294,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>4</v>
@@ -3990,7 +4305,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>4</v>
@@ -4001,7 +4316,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>4</v>
@@ -4012,7 +4327,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>4</v>
@@ -4023,7 +4338,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>4</v>
@@ -4034,18 +4349,18 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>238</v>
+        <v>290</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>4</v>
@@ -4056,7 +4371,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>4</v>
@@ -4067,18 +4382,18 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>238</v>
+        <v>291</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>4</v>
@@ -4089,7 +4404,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>4</v>
@@ -4100,7 +4415,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>4</v>
@@ -4111,7 +4426,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>4</v>
@@ -4129,8 +4444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F5617F-48D3-40DF-AB8B-773C68BA1F29}">
   <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView topLeftCell="A101" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4153,7 +4468,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -4164,7 +4479,7 @@
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -4175,7 +4490,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -4186,7 +4501,7 @@
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -4197,7 +4512,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -4208,7 +4523,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
@@ -4219,7 +4534,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
@@ -4230,7 +4545,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
@@ -4241,7 +4556,7 @@
     </row>
     <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
@@ -4252,7 +4567,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -4263,7 +4578,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
@@ -4274,7 +4589,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
@@ -4285,7 +4600,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
@@ -4296,7 +4611,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
@@ -4307,7 +4622,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
@@ -4318,7 +4633,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>4</v>
@@ -4329,7 +4644,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>4</v>
@@ -4340,7 +4655,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>4</v>
@@ -4351,7 +4666,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>4</v>
@@ -4362,7 +4677,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>4</v>
@@ -4373,7 +4688,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>4</v>
@@ -4384,7 +4699,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>4</v>
@@ -4395,7 +4710,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>4</v>
@@ -4406,7 +4721,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>4</v>
@@ -4417,7 +4732,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>4</v>
@@ -4428,7 +4743,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>4</v>
@@ -4439,7 +4754,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>4</v>
@@ -4450,7 +4765,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>4</v>
@@ -4461,7 +4776,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>4</v>
@@ -4472,7 +4787,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>4</v>
@@ -4483,7 +4798,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>4</v>
@@ -4494,7 +4809,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>4</v>
@@ -4505,7 +4820,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>4</v>
@@ -4516,7 +4831,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>4</v>
@@ -4527,7 +4842,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>4</v>
@@ -4538,7 +4853,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>4</v>
@@ -4549,7 +4864,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>4</v>
@@ -4560,7 +4875,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>4</v>
@@ -4571,7 +4886,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>4</v>
@@ -4582,18 +4897,18 @@
     </row>
     <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>48</v>
+        <v>292</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>4</v>
@@ -4604,7 +4919,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>4</v>
@@ -4615,7 +4930,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>4</v>
@@ -4626,7 +4941,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>4</v>
@@ -4637,7 +4952,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>4</v>
@@ -4648,7 +4963,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>4</v>
@@ -4659,7 +4974,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>4</v>
@@ -4670,7 +4985,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>4</v>
@@ -4681,7 +4996,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>4</v>
@@ -4692,7 +5007,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>4</v>
@@ -4703,7 +5018,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>4</v>
@@ -4714,7 +5029,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>4</v>
@@ -4725,7 +5040,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>4</v>
@@ -4736,7 +5051,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>4</v>
@@ -4747,7 +5062,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>4</v>
@@ -4758,7 +5073,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>4</v>
@@ -4769,7 +5084,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>4</v>
@@ -4780,7 +5095,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>4</v>
@@ -4791,7 +5106,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>4</v>
@@ -4802,7 +5117,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>4</v>
@@ -4813,7 +5128,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>4</v>
@@ -4824,7 +5139,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>4</v>
@@ -4835,7 +5150,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>4</v>
@@ -4846,7 +5161,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>4</v>
@@ -4857,7 +5172,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>4</v>
@@ -4868,7 +5183,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>4</v>
@@ -4879,7 +5194,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>4</v>
@@ -4890,7 +5205,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>4</v>
@@ -4901,7 +5216,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>4</v>
@@ -4912,7 +5227,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>4</v>
@@ -4923,7 +5238,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>4</v>
@@ -4934,7 +5249,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>4</v>
@@ -4945,7 +5260,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>4</v>
@@ -4956,7 +5271,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>4</v>
@@ -4967,7 +5282,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>4</v>
@@ -4978,7 +5293,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>4</v>
@@ -4989,7 +5304,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>4</v>
@@ -5000,7 +5315,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>4</v>
@@ -5011,7 +5326,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>4</v>
@@ -5022,7 +5337,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>4</v>
@@ -5033,7 +5348,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>4</v>
@@ -5044,7 +5359,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>4</v>
@@ -5055,7 +5370,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>4</v>
@@ -5066,7 +5381,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>4</v>
@@ -5077,7 +5392,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>4</v>
@@ -5088,7 +5403,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>4</v>
@@ -5099,7 +5414,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>4</v>
@@ -5110,7 +5425,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>4</v>
@@ -5121,7 +5436,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>4</v>
@@ -5132,18 +5447,18 @@
     </row>
     <row r="91" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>117</v>
+        <v>293</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>4</v>
@@ -5154,7 +5469,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>4</v>
@@ -5165,7 +5480,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>4</v>
@@ -5176,7 +5491,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>4</v>
@@ -5187,7 +5502,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>4</v>
@@ -5198,7 +5513,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>4</v>
@@ -5209,7 +5524,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>4</v>
@@ -5220,7 +5535,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>4</v>
@@ -5231,7 +5546,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>4</v>
@@ -5242,7 +5557,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>4</v>
@@ -5253,7 +5568,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>4</v>
@@ -5264,7 +5579,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>4</v>
@@ -5275,7 +5590,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>4</v>
@@ -5286,7 +5601,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>4</v>
@@ -5297,7 +5612,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>4</v>
@@ -5308,18 +5623,18 @@
     </row>
     <row r="107" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B107" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>4</v>
@@ -5330,7 +5645,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>4</v>
@@ -5341,18 +5656,18 @@
     </row>
     <row r="110" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>114</v>
+        <v>290</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>4</v>
@@ -5363,7 +5678,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>4</v>
@@ -5374,7 +5689,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>4</v>
@@ -5385,7 +5700,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>4</v>
@@ -5396,7 +5711,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>4</v>
@@ -5407,7 +5722,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Made small formatting changes.
</commit_message>
<xml_diff>
--- a/alignment_manual_changes.xlsx
+++ b/alignment_manual_changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="202" documentId="8_{887E55CB-68F7-4C6E-B521-2A75E9DA7E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53C2A65E-9EDB-4E8A-A865-D710DB542CBD}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="8_{887E55CB-68F7-4C6E-B521-2A75E9DA7E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB5D97AE-6611-4DA3-A7E7-E14AD8C77DEB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="13800" xr2:uid="{B05F01D2-BAAD-4BCF-B583-27E4851AB6BB}"/>
+    <workbookView xWindow="3660" yWindow="3144" windowWidth="17280" windowHeight="9000" activeTab="2" xr2:uid="{B05F01D2-BAAD-4BCF-B583-27E4851AB6BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Family" sheetId="3" r:id="rId1"/>
@@ -1868,23 +1868,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1D177B-7F3C-499B-AB5A-90CDE1F63245}">
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="47" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="48" zoomScaleNormal="40" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
+      <selection pane="topRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="93.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="59.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="93.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="45.7109375" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="93.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="59.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="93.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1916,7 +1916,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -2037,7 +2037,7 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>43</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>44</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>45</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>46</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>47</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>48</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>49</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>50</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>51</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>52</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>53</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>54</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>55</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>56</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>57</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>58</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>59</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>60</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>61</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>62</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>63</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>64</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>65</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>66</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>67</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>68</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>69</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>70</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>71</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>72</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>73</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>74</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>75</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>76</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>77</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>78</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>79</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>80</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>81</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>82</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>83</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>84</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>85</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>86</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>87</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>88</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>89</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>90</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>91</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>92</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>93</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>94</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>95</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>96</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>97</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>98</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>99</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>100</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>101</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>102</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>103</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>104</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>105</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>106</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>107</v>
       </c>
@@ -3084,7 +3084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>108</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>109</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>110</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>111</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>112</v>
       </c>
@@ -3148,920 +3148,920 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0B20D4-1C93-42FE-B91A-B9F801D5DCE5}">
   <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+    <sheetView zoomScale="64" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" style="1" customWidth="1"/>
     <col min="2" max="2" width="57" style="2" customWidth="1"/>
-    <col min="3" max="3" width="62.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="62.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>130</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>133</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>134</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>136</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>138</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>142</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>143</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>144</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>145</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>146</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>147</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>148</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>149</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>150</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>151</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>152</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>153</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>154</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>155</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>156</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>157</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>159</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>160</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>161</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C46" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>162</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C47" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C48" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>165</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>166</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C51" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>167</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C52" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C53" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>170</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C55" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>171</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>172</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C57" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>173</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C58" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>174</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C59" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>175</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C60" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>176</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C61" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>177</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C62" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>178</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C64" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>180</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C65" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>181</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>182</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>183</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C68" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>184</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C69" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C70" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>186</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>187</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C72" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C73" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>189</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>190</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C75" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>191</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C76" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>192</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C77" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>193</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C78" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>194</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C79" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>195</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C80" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>196</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>197</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="C82" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>198</v>
       </c>
@@ -4072,366 +4072,366 @@
         <v>236</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>199</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>200</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C85" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>201</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C86" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>202</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C87" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>203</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C88" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>204</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C89" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>205</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C90" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>206</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C91" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>207</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C92" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>208</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C93" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>209</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C94" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>210</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C95" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>211</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C96" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>212</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C97" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>213</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C98" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>214</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C99" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>215</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C100" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>216</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C101" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>217</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C102" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>218</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C103" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>219</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C104" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>220</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C105" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>221</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C106" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>222</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C107" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>223</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C108" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>224</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C109" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>225</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C110" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>226</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C111" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C111" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>227</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C112" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>228</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C113" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>229</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C114" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>230</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C115" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C115" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>231</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C116" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4444,18 +4444,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F5617F-48D3-40DF-AB8B-773C68BA1F29}">
   <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B119" sqref="B119"/>
+    <sheetView tabSelected="1" zoomScale="45" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="77" style="1" customWidth="1"/>
-    <col min="3" max="3" width="59.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="59.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>117</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>118</v>
       </c>
@@ -4488,7 +4488,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>119</v>
       </c>
@@ -4499,7 +4499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>120</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>121</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>122</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>123</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>124</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>125</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>126</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>127</v>
       </c>
@@ -4587,7 +4587,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>128</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>129</v>
       </c>
@@ -4609,7 +4609,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>130</v>
       </c>
@@ -4620,7 +4620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>131</v>
       </c>
@@ -4631,7 +4631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>132</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>133</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>134</v>
       </c>
@@ -4664,7 +4664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>135</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>136</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>137</v>
       </c>
@@ -4697,7 +4697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>138</v>
       </c>
@@ -4708,7 +4708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>139</v>
       </c>
@@ -4719,7 +4719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>140</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>141</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>142</v>
       </c>
@@ -4752,7 +4752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>143</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>144</v>
       </c>
@@ -4774,7 +4774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>145</v>
       </c>
@@ -4785,7 +4785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>146</v>
       </c>
@@ -4796,7 +4796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>147</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>148</v>
       </c>
@@ -4818,7 +4818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>149</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>150</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>151</v>
       </c>
@@ -4851,7 +4851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>152</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>153</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>154</v>
       </c>
@@ -4884,7 +4884,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>155</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>156</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>157</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>158</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>159</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>160</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>161</v>
       </c>
@@ -4961,7 +4961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>162</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>163</v>
       </c>
@@ -4983,7 +4983,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>164</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>165</v>
       </c>
@@ -5005,7 +5005,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>166</v>
       </c>
@@ -5016,7 +5016,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>167</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>168</v>
       </c>
@@ -5038,7 +5038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>169</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>170</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>171</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>172</v>
       </c>
@@ -5082,7 +5082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>173</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>174</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>175</v>
       </c>
@@ -5115,7 +5115,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>176</v>
       </c>
@@ -5126,7 +5126,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>177</v>
       </c>
@@ -5137,7 +5137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>178</v>
       </c>
@@ -5148,7 +5148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>179</v>
       </c>
@@ -5159,7 +5159,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>180</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>181</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>182</v>
       </c>
@@ -5192,7 +5192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>183</v>
       </c>
@@ -5203,7 +5203,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>184</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>185</v>
       </c>
@@ -5225,7 +5225,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>186</v>
       </c>
@@ -5236,7 +5236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>187</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>188</v>
       </c>
@@ -5258,7 +5258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>189</v>
       </c>
@@ -5269,7 +5269,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>190</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>191</v>
       </c>
@@ -5291,7 +5291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>192</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>193</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>194</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>195</v>
       </c>
@@ -5335,7 +5335,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>196</v>
       </c>
@@ -5346,7 +5346,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>197</v>
       </c>
@@ -5357,7 +5357,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>198</v>
       </c>
@@ -5368,7 +5368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>199</v>
       </c>
@@ -5379,7 +5379,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>200</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>201</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>202</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>203</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>204</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>205</v>
       </c>
@@ -5445,7 +5445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>206</v>
       </c>
@@ -5456,7 +5456,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>207</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>208</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>209</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>210</v>
       </c>
@@ -5500,7 +5500,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>211</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>212</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>213</v>
       </c>
@@ -5533,7 +5533,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>214</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>215</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>216</v>
       </c>
@@ -5566,7 +5566,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>217</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>218</v>
       </c>
@@ -5588,7 +5588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>219</v>
       </c>
@@ -5599,7 +5599,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>220</v>
       </c>
@@ -5610,7 +5610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>221</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>222</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>223</v>
       </c>
@@ -5643,7 +5643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>224</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>225</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>226</v>
       </c>
@@ -5676,7 +5676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>227</v>
       </c>
@@ -5687,7 +5687,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>228</v>
       </c>
@@ -5698,7 +5698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>229</v>
       </c>
@@ -5709,7 +5709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>230</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>231</v>
       </c>

</xml_diff>

<commit_message>
Updates following the identification of additional genes to remove from family and genus-level concatonated analyses due to scoring 'TRUE' against Criteria A
</commit_message>
<xml_diff>
--- a/alignment_manual_changes.xlsx
+++ b/alignment_manual_changes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{B7244E2E-A750-43FF-874D-10FA35632DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD5A6E20-0B4B-4B55-BC3D-A75ABC5B76CF}"/>
   <bookViews>
-    <workbookView xWindow="132" yWindow="3264" windowWidth="21528" windowHeight="10308" xr2:uid="{B05F01D2-BAAD-4BCF-B583-27E4851AB6BB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B05F01D2-BAAD-4BCF-B583-27E4851AB6BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Family" sheetId="3" r:id="rId1"/>
@@ -1694,23 +1694,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1D177B-7F3C-499B-AB5A-90CDE1F63245}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="71" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="40" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="B32" sqref="B32"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="93.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="59.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="93.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="45.6640625" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="38.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="93.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="59.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="93.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1863,7 +1863,7 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -2160,18 +2160,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0B20D4-1C93-42FE-B91A-B9F801D5DCE5}">
   <dimension ref="A1:C117"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScale="50" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView zoomScale="50" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" style="1" customWidth="1"/>
     <col min="2" max="2" width="57" style="2" customWidth="1"/>
-    <col min="3" max="3" width="62.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="62.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>53</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>56</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>57</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>59</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>60</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>61</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>64</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>67</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>68</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>69</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>70</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>71</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>73</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>74</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>75</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>76</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>77</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>78</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>79</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>80</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>81</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>82</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>83</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>85</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>86</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>87</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>88</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>89</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>90</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>91</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>92</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>93</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>94</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>95</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>96</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>97</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>98</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>99</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>100</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>101</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>102</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>103</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>104</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>105</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>106</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>107</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>108</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>109</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>110</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>111</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>112</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>113</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>114</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>115</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>116</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>117</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>118</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>119</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>120</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>121</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>122</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>123</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>124</v>
       </c>
@@ -3084,7 +3084,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>125</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>126</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>127</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>128</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>129</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>130</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>131</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>132</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>133</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>134</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>135</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>136</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>137</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>138</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>139</v>
       </c>
@@ -3249,7 +3249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>140</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>141</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>142</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>143</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>144</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>145</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>146</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>147</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>148</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>149</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>150</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>151</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>152</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>153</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>154</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>155</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>156</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>157</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>221</v>
       </c>
@@ -3468,18 +3468,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F5617F-48D3-40DF-AB8B-773C68BA1F29}">
   <dimension ref="A1:C117"/>
   <sheetViews>
-    <sheetView zoomScale="73" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView topLeftCell="A88" zoomScale="73" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="77" style="1" customWidth="1"/>
-    <col min="3" max="3" width="59.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="59.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
@@ -3545,7 +3545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>53</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>56</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>57</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>59</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>60</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>61</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>64</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>67</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>68</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>69</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>70</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>71</v>
       </c>
@@ -3809,7 +3809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>73</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>74</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>75</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>76</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>77</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>78</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>79</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>80</v>
       </c>
@@ -3908,7 +3908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>81</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>82</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>83</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>85</v>
       </c>
@@ -3963,7 +3963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>86</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>87</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>88</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>89</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>90</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>91</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>92</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>93</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>94</v>
       </c>
@@ -4062,7 +4062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>95</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>96</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>97</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>98</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>99</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>100</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>101</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>102</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>103</v>
       </c>
@@ -4161,7 +4161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>104</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>105</v>
       </c>
@@ -4183,7 +4183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>106</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>107</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>108</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>109</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>110</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>111</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>112</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>113</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>114</v>
       </c>
@@ -4282,7 +4282,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>115</v>
       </c>
@@ -4293,7 +4293,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>116</v>
       </c>
@@ -4304,7 +4304,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>117</v>
       </c>
@@ -4315,7 +4315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>118</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>119</v>
       </c>
@@ -4337,7 +4337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>120</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>121</v>
       </c>
@@ -4359,7 +4359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>122</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>123</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>124</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>125</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>126</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>127</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>128</v>
       </c>
@@ -4436,7 +4436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>129</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>130</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>131</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>132</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>133</v>
       </c>
@@ -4491,7 +4491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>134</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>135</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>136</v>
       </c>
@@ -4524,7 +4524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>137</v>
       </c>
@@ -4535,7 +4535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>138</v>
       </c>
@@ -4546,7 +4546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>139</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>140</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>141</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>142</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>143</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>144</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>145</v>
       </c>
@@ -4623,7 +4623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>146</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>147</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>148</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>149</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>150</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>151</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>152</v>
       </c>
@@ -4700,7 +4700,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>153</v>
       </c>
@@ -4711,7 +4711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>154</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>155</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>156</v>
       </c>
@@ -4744,7 +4744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>157</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>221</v>
       </c>

</xml_diff>

<commit_message>
Updates after proofreading and updating script numbers.
</commit_message>
<xml_diff>
--- a/alignment_manual_changes.xlsx
+++ b/alignment_manual_changes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{B7244E2E-A750-43FF-874D-10FA35632DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD5A6E20-0B4B-4B55-BC3D-A75ABC5B76CF}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{B7244E2E-A750-43FF-874D-10FA35632DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51D7E8BE-09D5-4927-B463-0A2E19365EDD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B05F01D2-BAAD-4BCF-B583-27E4851AB6BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{B05F01D2-BAAD-4BCF-B583-27E4851AB6BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Family" sheetId="3" r:id="rId1"/>
@@ -1694,23 +1694,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1D177B-7F3C-499B-AB5A-90CDE1F63245}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScale="71" zoomScaleNormal="40" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3"/>
+      <selection pane="topRight" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="93.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="59.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="93.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="45.7109375" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="93.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="59.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="93.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1863,7 +1863,7 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -2160,18 +2160,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0B20D4-1C93-42FE-B91A-B9F801D5DCE5}">
   <dimension ref="A1:C117"/>
   <sheetViews>
-    <sheetView zoomScale="50" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" style="1" customWidth="1"/>
-    <col min="2" max="2" width="57" style="2" customWidth="1"/>
-    <col min="3" max="3" width="62.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="91.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="62.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>53</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>56</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>57</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>59</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>60</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>61</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>64</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>67</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>68</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>69</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>70</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>71</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>73</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>74</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>75</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>76</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>77</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>78</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>79</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>80</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>81</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>82</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>83</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>85</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>86</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>87</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>88</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>89</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>90</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>91</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>92</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>93</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>94</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>95</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>96</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>97</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>98</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>99</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>100</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>101</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>102</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>103</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>104</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>105</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>106</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>107</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>108</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>109</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>110</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>111</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>112</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>113</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>114</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>115</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>116</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>117</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>118</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>119</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>120</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>121</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>122</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>123</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>124</v>
       </c>
@@ -3084,7 +3084,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>125</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>126</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>127</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>128</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>129</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>130</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>131</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>132</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>133</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>134</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>135</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>136</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>137</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>138</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>139</v>
       </c>
@@ -3249,7 +3249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>140</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>141</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>142</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>143</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>144</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>145</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>146</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>147</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>148</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>149</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>150</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>151</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>152</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>153</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>154</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>155</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>156</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>157</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>221</v>
       </c>
@@ -3472,14 +3472,14 @@
       <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="77" style="1" customWidth="1"/>
-    <col min="3" max="3" width="59.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="59.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
@@ -3545,7 +3545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>53</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>56</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>57</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>59</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>60</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>61</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>64</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>67</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>68</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>69</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>70</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>71</v>
       </c>
@@ -3809,7 +3809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>73</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>74</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>75</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>76</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>77</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>78</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>79</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>80</v>
       </c>
@@ -3908,7 +3908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>81</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>82</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>83</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>85</v>
       </c>
@@ -3963,7 +3963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>86</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>87</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>88</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>89</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>90</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>91</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>92</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>93</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>94</v>
       </c>
@@ -4062,7 +4062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>95</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>96</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>97</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>98</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>99</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>100</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>101</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>102</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>103</v>
       </c>
@@ -4161,7 +4161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>104</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>105</v>
       </c>
@@ -4183,7 +4183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>106</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>107</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>108</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>109</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>110</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>111</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>112</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>113</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>114</v>
       </c>
@@ -4282,7 +4282,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>115</v>
       </c>
@@ -4293,7 +4293,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>116</v>
       </c>
@@ -4304,7 +4304,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>117</v>
       </c>
@@ -4315,7 +4315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>118</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>119</v>
       </c>
@@ -4337,7 +4337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>120</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>121</v>
       </c>
@@ -4359,7 +4359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>122</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>123</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>124</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>125</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>126</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>127</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>128</v>
       </c>
@@ -4436,7 +4436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>129</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>130</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>131</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>132</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>133</v>
       </c>
@@ -4491,7 +4491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>134</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>135</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>136</v>
       </c>
@@ -4524,7 +4524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>137</v>
       </c>
@@ -4535,7 +4535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>138</v>
       </c>
@@ -4546,7 +4546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>139</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>140</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>141</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>142</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>143</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>144</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>145</v>
       </c>
@@ -4623,7 +4623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>146</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>147</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>148</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>149</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>150</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>151</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>152</v>
       </c>
@@ -4700,7 +4700,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>153</v>
       </c>
@@ -4711,7 +4711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>154</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>155</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>156</v>
       </c>
@@ -4744,7 +4744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>157</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>221</v>
       </c>

</xml_diff>